<commit_message>
fixed issue of suzuki austrelia
</commit_message>
<xml_diff>
--- a/output/61bbdb19-1f94-4617-8814-9148f0a43000/61bbdb19-1f94-4617-8814-9148f0a43000_main_pages.xlsx
+++ b/output/61bbdb19-1f94-4617-8814-9148f0a43000/61bbdb19-1f94-4617-8814-9148f0a43000_main_pages.xlsx
@@ -688,6 +688,12 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
       <c r="E2" t="s">
         <v>46</v>
       </c>
@@ -776,6 +782,12 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
       <c r="E7" t="s">
         <v>46</v>
       </c>
@@ -881,6 +893,12 @@
       <c r="A13" t="s">
         <v>15</v>
       </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
       <c r="E13" t="s">
         <v>47</v>
       </c>
@@ -1029,6 +1047,12 @@
       <c r="A21" t="s">
         <v>23</v>
       </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
       <c r="E21" t="s">
         <v>47</v>
       </c>
@@ -1190,6 +1214,12 @@
     <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>28</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
       </c>
       <c r="E30" t="s">
         <v>47</v>
@@ -1463,6 +1493,12 @@
       <c r="A17" t="s">
         <v>66</v>
       </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
@@ -1512,6 +1548,12 @@
       <c r="A2" t="s">
         <v>72</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
       <c r="E2" t="s">
         <v>92</v>
       </c>
@@ -1593,6 +1635,12 @@
       <c r="A8" t="s">
         <v>78</v>
       </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
       <c r="E8" t="s">
         <v>93</v>
       </c>
@@ -1657,6 +1705,12 @@
       <c r="A13" t="s">
         <v>83</v>
       </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
       <c r="E13" t="s">
         <v>94</v>
       </c>
@@ -1665,6 +1719,9 @@
       <c r="A14" t="s">
         <v>84</v>
       </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
       <c r="D14">
         <v>3000</v>
       </c>
@@ -1675,6 +1732,9 @@
     <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>85</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
       </c>
       <c r="D15">
         <v>-13000</v>

</xml_diff>